<commit_message>
Fix weights bug in XlsxFileIO
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/meetingscheduling/unsolved/100meetings-320timegrains-5rooms.xlsx
+++ b/optaplanner-examples/data/meetingscheduling/unsolved/100meetings-320timegrains-5rooms.xlsx
@@ -21,7 +21,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26613" uniqueCount="514">
   <si>
-    <t>Fri 2018-10-05 13:50</t>
+    <t>Wed 2018-10-10 16:04</t>
   </si>
   <si>
     <t>Constraint</t>
@@ -1582,7 +1582,7 @@
       <b val="true"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1617,6 +1617,11 @@
         <fgColor rgb="FCAF3E"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1630,7 +1635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment wrapText="true" vertical="center"/>
@@ -1654,6 +1659,9 @@
       <alignment wrapText="true" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true">
       <alignment wrapText="true" vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>